<commit_message>
Refactorization + user input on workout primacy
</commit_message>
<xml_diff>
--- a/Exercises.xlsx
+++ b/Exercises.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ageary\Documents\Personal\Github\workout-picker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71303ADB-FCA3-46FF-8E59-ADC84BFB9707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE9C76B-276B-464C-95D5-0F46916F04EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{08033872-2FC8-4F56-87A7-576AB28DC7B9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Exercises" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Exercises!$A$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Exercises!$A$1:$G$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="37">
   <si>
     <t>upper_lower</t>
   </si>
@@ -115,24 +115,6 @@
     <t>push</t>
   </si>
   <si>
-    <t>aux</t>
-  </si>
-  <si>
-    <t>vertical push</t>
-  </si>
-  <si>
-    <t>vertical pull</t>
-  </si>
-  <si>
-    <t>horizontal pull</t>
-  </si>
-  <si>
-    <t>horizontal push</t>
-  </si>
-  <si>
-    <t>horiztonal push</t>
-  </si>
-  <si>
     <t>run</t>
   </si>
   <si>
@@ -143,6 +125,30 @@
   </si>
   <si>
     <t>ab wheel + leg raises + flutter kicks</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>horizontal</t>
+  </si>
+  <si>
+    <t>vertical</t>
+  </si>
+  <si>
+    <t>hang clean</t>
+  </si>
+  <si>
+    <t>primacy</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>primary</t>
   </si>
 </sst>
 </file>
@@ -525,385 +531,544 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C84E1D-B242-416A-82FE-C6DDE98D13D1}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="E19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
+      <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1048576" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{13C84E1D-B242-416A-82FE-C6DDE98D13D1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
-      <sortCondition ref="B1:B12"/>
+  <autoFilter ref="A1:G12" xr:uid="{13C84E1D-B242-416A-82FE-C6DDE98D13D1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+      <sortCondition ref="C1:C12"/>
     </sortState>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G22">
+    <sortCondition ref="C2:C22"/>
+    <sortCondition ref="D2:D22"/>
+    <sortCondition ref="E2:E22"/>
+    <sortCondition descending="1" ref="G2:G22"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>